<commit_message>
glucose model mass and charge balanced
</commit_message>
<xml_diff>
--- a/python/multiscalepy/multiscale/modelcreator/models/glucose/glucose_annotations.xlsx
+++ b/python/multiscalepy/multiscale/modelcreator/models/glucose/glucose_annotations.xlsx
@@ -941,6 +941,60 @@
     <t>HO7P2</t>
   </si>
   <si>
+    <t>^co2[_]*\w*$</t>
+  </si>
+  <si>
+    <t>CHEBI:16526</t>
+  </si>
+  <si>
+    <t>carbon dioxide</t>
+  </si>
+  <si>
+    <t>C00011</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>^h[_]*\w*$</t>
+  </si>
+  <si>
+    <t>CHEBI:15378</t>
+  </si>
+  <si>
+    <t>hydron</t>
+  </si>
+  <si>
+    <t>C00080</t>
+  </si>
+  <si>
+    <t>H+</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>^h2[_]*\w*$</t>
+  </si>
+  <si>
+    <t>CHEBI:18276</t>
+  </si>
+  <si>
+    <t>dihydrogen</t>
+  </si>
+  <si>
+    <t>C00282</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
     <t>^h2o[_]*\w*$</t>
   </si>
   <si>
@@ -954,60 +1008,6 @@
   </si>
   <si>
     <t>H2O</t>
-  </si>
-  <si>
-    <t>^co2[_]*\w*$</t>
-  </si>
-  <si>
-    <t>CHEBI:16526</t>
-  </si>
-  <si>
-    <t>carbon dioxide</t>
-  </si>
-  <si>
-    <t>C00011</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>^h[_]*\w*$</t>
-  </si>
-  <si>
-    <t>CHEBI:15378</t>
-  </si>
-  <si>
-    <t>hydron</t>
-  </si>
-  <si>
-    <t>C00080</t>
-  </si>
-  <si>
-    <t>H+</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>+1</t>
-  </si>
-  <si>
-    <t>^h2[_]*\w*$</t>
-  </si>
-  <si>
-    <t>CHEBI:18276</t>
-  </si>
-  <si>
-    <t>dihydrogen</t>
-  </si>
-  <si>
-    <t>C00282</t>
-  </si>
-  <si>
-    <t>Hydrogen</t>
-  </si>
-  <si>
-    <t>H2</t>
   </si>
   <si>
     <t>^glc1p[_]*\w*$</t>
@@ -1566,8 +1566,8 @@
   </sheetPr>
   <dimension ref="A1:G457"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A412" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D453" activeCellId="0" sqref="D453"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A307" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A318" activeCellId="0" sqref="A318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7761,7 +7761,7 @@
         <v>238</v>
       </c>
       <c r="D327" s="13" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E327" s="7"/>
       <c r="F327" s="7"/>
@@ -7778,24 +7778,24 @@
         <v>240</v>
       </c>
       <c r="D328" s="11" t="s">
-        <v>241</v>
+        <v>319</v>
       </c>
       <c r="E328" s="7"/>
       <c r="F328" s="7"/>
       <c r="G328" s="0"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="0"/>
-      <c r="B329" s="0"/>
-      <c r="C329" s="0"/>
-      <c r="D329" s="15"/>
-      <c r="E329" s="0"/>
-      <c r="F329" s="0"/>
+      <c r="A329" s="14"/>
+      <c r="B329" s="7"/>
+      <c r="C329" s="7"/>
+      <c r="D329" s="11"/>
+      <c r="E329" s="7"/>
+      <c r="F329" s="7"/>
       <c r="G329" s="0"/>
     </row>
     <row r="330" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="14" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B330" s="7" t="s">
         <v>231</v>
@@ -7818,7 +7818,7 @@
     </row>
     <row r="331" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="14" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B331" s="7" t="s">
         <v>231</v>
@@ -7827,7 +7827,7 @@
         <v>11</v>
       </c>
       <c r="D331" s="11" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E331" s="7" t="s">
         <v>22</v>
@@ -7836,12 +7836,12 @@
         <v>90</v>
       </c>
       <c r="G331" s="12" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="14" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B332" s="7" t="s">
         <v>231</v>
@@ -7850,7 +7850,7 @@
         <v>11</v>
       </c>
       <c r="D332" s="11" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E332" s="7" t="s">
         <v>22</v>
@@ -7859,12 +7859,12 @@
         <v>92</v>
       </c>
       <c r="G332" s="12" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="14" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B333" s="7" t="s">
         <v>231</v>
@@ -7873,7 +7873,7 @@
         <v>238</v>
       </c>
       <c r="D333" s="13" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E333" s="7"/>
       <c r="F333" s="7"/>
@@ -7881,7 +7881,7 @@
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="14" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B334" s="7" t="s">
         <v>231</v>
@@ -7890,7 +7890,7 @@
         <v>240</v>
       </c>
       <c r="D334" s="11" t="s">
-        <v>324</v>
+        <v>241</v>
       </c>
       <c r="E334" s="7"/>
       <c r="F334" s="7"/>
@@ -7907,7 +7907,7 @@
     </row>
     <row r="336" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B336" s="7" t="s">
         <v>231</v>
@@ -7930,7 +7930,7 @@
     </row>
     <row r="337" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B337" s="7" t="s">
         <v>231</v>
@@ -7939,7 +7939,7 @@
         <v>11</v>
       </c>
       <c r="D337" s="11" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E337" s="7" t="s">
         <v>22</v>
@@ -7948,12 +7948,12 @@
         <v>90</v>
       </c>
       <c r="G337" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B338" s="7" t="s">
         <v>231</v>
@@ -7962,7 +7962,7 @@
         <v>11</v>
       </c>
       <c r="D338" s="11" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E338" s="7" t="s">
         <v>22</v>
@@ -7971,12 +7971,12 @@
         <v>92</v>
       </c>
       <c r="G338" s="12" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B339" s="7" t="s">
         <v>231</v>
@@ -7993,7 +7993,7 @@
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B340" s="7" t="s">
         <v>231</v>
@@ -8017,7 +8017,7 @@
       <c r="F341" s="0"/>
       <c r="G341" s="0"/>
     </row>
-    <row r="342" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="14" t="s">
         <v>331</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="343" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="14" t="s">
         <v>331</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="14" t="s">
         <v>331</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="14" t="s">
         <v>331</v>
       </c>
@@ -8129,7 +8129,7 @@
       <c r="F347" s="0"/>
       <c r="G347" s="0"/>
     </row>
-    <row r="348" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="14" t="s">
         <v>337</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="14" t="s">
         <v>337</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="14" t="s">
         <v>337</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="14" t="s">
         <v>337</v>
       </c>
@@ -8241,7 +8241,7 @@
       <c r="F353" s="0"/>
       <c r="G353" s="0"/>
     </row>
-    <row r="354" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="14" t="s">
         <v>343</v>
       </c>
@@ -8349,7 +8349,7 @@
       <c r="F359" s="0"/>
       <c r="G359" s="0"/>
     </row>
-    <row r="360" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="14" t="s">
         <v>346</v>
       </c>
@@ -8372,7 +8372,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="14" t="s">
         <v>346</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="14" t="s">
         <v>346</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="14" t="s">
         <v>346</v>
       </c>
@@ -8461,7 +8461,7 @@
       <c r="F365" s="0"/>
       <c r="G365" s="0"/>
     </row>
-    <row r="366" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="14" t="s">
         <v>351</v>
       </c>
@@ -8505,7 +8505,7 @@
       </c>
       <c r="G367" s="0"/>
     </row>
-    <row r="368" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="14" t="s">
         <v>351</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="369" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="14" t="s">
         <v>351</v>
       </c>
@@ -8571,7 +8571,7 @@
       <c r="F371" s="0"/>
       <c r="G371" s="0"/>
     </row>
-    <row r="372" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="14" t="s">
         <v>355</v>
       </c>
@@ -8638,7 +8638,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="375" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="14" t="s">
         <v>355</v>
       </c>
@@ -8681,7 +8681,7 @@
       <c r="F377" s="0"/>
       <c r="G377" s="0"/>
     </row>
-    <row r="378" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="14" t="s">
         <v>360</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="429" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="14" t="s">
         <v>397</v>
       </c>
@@ -9738,7 +9738,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="435" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="14" t="s">
         <v>402</v>
       </c>
@@ -9781,7 +9781,7 @@
       <c r="F437" s="7"/>
       <c r="G437" s="0"/>
     </row>
-    <row r="438" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="14" t="s">
         <v>407</v>
       </c>

</xml_diff>

<commit_message>
Fixed rule SBO terms and annotations
</commit_message>
<xml_diff>
--- a/python/multiscalepy/multiscale/modelcreator/models/glucose/glucose_annotations.xlsx
+++ b/python/multiscalepy/multiscale/modelcreator/models/glucose/glucose_annotations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="427">
   <si>
     <t>pattern</t>
   </si>
@@ -1287,6 +1287,9 @@
   </si>
   <si>
     <t>^[\w_]*_tot$</t>
+  </si>
+  <si>
+    <t>rule</t>
   </si>
   <si>
     <t>SBO:0000359</t>
@@ -1566,8 +1569,8 @@
   </sheetPr>
   <dimension ref="A1:G457"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A307" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A318" activeCellId="0" sqref="A318"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A451" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B457" activeCellId="0" sqref="B457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10127,13 +10130,13 @@
         <v>423</v>
       </c>
       <c r="B457" s="7" t="s">
-        <v>73</v>
+        <v>424</v>
       </c>
       <c r="C457" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D457" s="13" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E457" s="7" t="s">
         <v>22</v>
@@ -10142,7 +10145,7 @@
         <v>14</v>
       </c>
       <c r="G457" s="12" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>